<commit_message>
update + add providers
</commit_message>
<xml_diff>
--- a/public/templates/books_ex.xlsx
+++ b/public/templates/books_ex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\library_invoices\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E48D39C-C2B2-4F79-850E-754959179C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8A8F21-ED5F-411F-B1A7-1557D4555C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>سعر الشراء</t>
   </si>
   <si>
-    <t>سعر البيع</t>
-  </si>
-  <si>
     <t>أحمد المراد</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>الضامري</t>
+  </si>
+  <si>
+    <t>نسبة البيع (%)</t>
   </si>
 </sst>
 </file>
@@ -457,18 +457,19 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="58" style="1" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" style="1" customWidth="1"/>
     <col min="2" max="4" width="18.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -502,30 +503,30 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="1">
         <v>2018</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1">
         <v>7</v>
@@ -534,7 +535,7 @@
         <v>270</v>
       </c>
       <c r="J2" s="1">
-        <v>351</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1">
         <v>1</v>
@@ -542,25 +543,25 @@
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1">
         <v>2007</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1">
         <v>22</v>
@@ -569,7 +570,7 @@
         <v>230</v>
       </c>
       <c r="J3" s="1">
-        <v>350</v>
+        <v>25</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
schedule tasks, offline fonts
</commit_message>
<xml_diff>
--- a/public/templates/books_ex.xlsx
+++ b/public/templates/books_ex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\library_invoices\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C4DB92-45BA-40A6-9DBC-E89ED158463A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB08FDF-E4F9-4C81-9F7E-D7632635C58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -578,13 +578,20 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{B3255F1A-9BA7-4417-A66D-AC5C9ED5EE3F}">
+  <dataValidations count="4">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="انتبه" error="أدخل القيمة 0 أو 1 فقط حسب الحالة." promptTitle="ملاحظة" prompt="إن كان التخفيض ممكنا أدخل القيمة 1 ، وإن كان غير ممكن أدخل القيمة 0." sqref="K1:K1048576" xr:uid="{5E6CE7F9-0868-487B-876D-7758BF5254B2}">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="انتبه" error="يجب أن تكون نسبة البيع ضمن القيم: [0 , 10, 15, 20, 25, 30]" promptTitle="ملاحظة" prompt="أدخل نسبة البيع من القيم: [0 , 10, 15, 20, 25, 30] " sqref="J1:J1048576" xr:uid="{522A1A9D-545D-4B60-9711-73FF33994AD4}">
       <formula1>"0,10,15,20,25,30"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="J1 K1" xr:uid="{DB44B146-91E6-42C5-AEE4-288307B68DDF}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{9FFD26E7-2F6B-4246-942B-214CB8B01350}">
-      <formula1>"0,1"</formula1>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{A965A763-6B8D-480B-AC61-D7E2DC2C7351}">
+      <formula1>0</formula1>
+      <formula2>100000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{83763F8A-6FB2-447B-A643-D42B22E3BE42}">
+      <formula1>0</formula1>
+      <formula2>3000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>